<commit_message>
Sign up screen dan akses database
</commit_message>
<xml_diff>
--- a/Converter.xlsx
+++ b/Converter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\CoffeeTime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2C6C062-C077-4FC1-A3E2-869092D57563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5A2700-5D3E-4D18-B27F-1CA40C6ED09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{828984FF-DB3C-40B6-9A60-DC5481C5CA00}"/>
   </bookViews>

</xml_diff>